<commit_message>
update trophy and problem animal
</commit_message>
<xml_diff>
--- a/data/HUNT_STATS_LIMPOPO_15.04.16.xlsx
+++ b/data/HUNT_STATS_LIMPOPO_15.04.16.xlsx
@@ -9,15 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="raw.data" sheetId="1" r:id="rId1"/>
+    <sheet name="summary" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw.data!$A$1:$E$132</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="5" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="170">
   <si>
     <t>2014_1</t>
   </si>
@@ -525,6 +529,21 @@
   </si>
   <si>
     <t>11</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Count of hunt.successful</t>
+  </si>
+  <si>
+    <t>(Multiple Items)</t>
   </si>
 </sst>
 </file>
@@ -566,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -585,6 +604,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,6 +621,1105 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ross Pitman" refreshedDate="42479.594571180554" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="132">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:E1048576" sheet="raw.data"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="year" numFmtId="49">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2013" maxValue="2015" count="4">
+        <n v="2013"/>
+        <n v="2014"/>
+        <n v="2015"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="year.id" numFmtId="49">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="hunt.successful" numFmtId="49">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="2" count="5">
+        <n v="1"/>
+        <n v="2"/>
+        <s v="1"/>
+        <s v="2"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="time.to.kill" numFmtId="49">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="21"/>
+    </cacheField>
+    <cacheField name="age.class" numFmtId="49">
+      <sharedItems containsBlank="1" count="12">
+        <s v="ADULT"/>
+        <s v="NA"/>
+        <s v="ADULT &lt;7 YRS"/>
+        <s v="ADULT &gt;7 YRS"/>
+        <s v="SUBADULT"/>
+        <s v="ADULT&lt;7 YRS"/>
+        <s v="MALE ADULT &lt;7"/>
+        <s v="FEMALE ADULT"/>
+        <s v="FEMALE SUBADULT"/>
+        <s v="MALE ADULT &gt;7"/>
+        <s v="MALE SUBADULT"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="132">
+  <r>
+    <x v="0"/>
+    <s v="2013_1"/>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_2"/>
+    <x v="0"/>
+    <n v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_3"/>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_4"/>
+    <x v="0"/>
+    <n v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_5"/>
+    <x v="0"/>
+    <n v="7"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_6"/>
+    <x v="0"/>
+    <n v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_7"/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_8"/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_9"/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_10"/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_11"/>
+    <x v="0"/>
+    <n v="13"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_12"/>
+    <x v="0"/>
+    <n v="5"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_13"/>
+    <x v="0"/>
+    <n v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_14"/>
+    <x v="0"/>
+    <n v="3"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_15"/>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_16"/>
+    <x v="0"/>
+    <n v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_17"/>
+    <x v="0"/>
+    <n v="16"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_18"/>
+    <x v="0"/>
+    <n v="3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_19"/>
+    <x v="0"/>
+    <n v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_20"/>
+    <x v="0"/>
+    <n v="13"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_21"/>
+    <x v="0"/>
+    <n v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_22"/>
+    <x v="0"/>
+    <n v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_23"/>
+    <x v="0"/>
+    <n v="6"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_24"/>
+    <x v="0"/>
+    <n v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_25"/>
+    <x v="0"/>
+    <n v="7"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_26"/>
+    <x v="0"/>
+    <n v="2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_27"/>
+    <x v="0"/>
+    <n v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_28"/>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_29"/>
+    <x v="0"/>
+    <n v="4"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_30"/>
+    <x v="0"/>
+    <n v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_31"/>
+    <x v="0"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="2013_32"/>
+    <x v="0"/>
+    <n v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_1"/>
+    <x v="2"/>
+    <s v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_2"/>
+    <x v="3"/>
+    <s v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_3"/>
+    <x v="2"/>
+    <s v="12"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_4"/>
+    <x v="3"/>
+    <s v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_5"/>
+    <x v="2"/>
+    <s v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_6"/>
+    <x v="2"/>
+    <s v="5"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_7"/>
+    <x v="2"/>
+    <s v="10"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_8"/>
+    <x v="2"/>
+    <s v="12"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_9"/>
+    <x v="2"/>
+    <s v="8"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_10"/>
+    <x v="2"/>
+    <s v="2"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_11"/>
+    <x v="2"/>
+    <s v="8"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_12"/>
+    <x v="2"/>
+    <s v="6"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_13"/>
+    <x v="0"/>
+    <n v="3"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_14"/>
+    <x v="0"/>
+    <n v="18"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_15"/>
+    <x v="0"/>
+    <n v="13"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_16"/>
+    <x v="0"/>
+    <n v="6"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_17"/>
+    <x v="0"/>
+    <n v="2"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_18"/>
+    <x v="0"/>
+    <n v="2"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_19"/>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_20"/>
+    <x v="0"/>
+    <n v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_21"/>
+    <x v="0"/>
+    <n v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_22"/>
+    <x v="0"/>
+    <n v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_23"/>
+    <x v="0"/>
+    <n v="12"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_24"/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_25"/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_26"/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_27"/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_28"/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_29"/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_30"/>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_31"/>
+    <x v="0"/>
+    <n v="4"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_32"/>
+    <x v="0"/>
+    <n v="6"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_33"/>
+    <x v="0"/>
+    <n v="10"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_34"/>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_35"/>
+    <x v="0"/>
+    <n v="3"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_36"/>
+    <x v="0"/>
+    <n v="4"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_37"/>
+    <x v="0"/>
+    <n v="3"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_38"/>
+    <x v="0"/>
+    <n v="3"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_39"/>
+    <x v="0"/>
+    <n v="3"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_40"/>
+    <x v="0"/>
+    <n v="10"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_41"/>
+    <x v="0"/>
+    <n v="7"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_42"/>
+    <x v="0"/>
+    <n v="2"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_43"/>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_44"/>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_45"/>
+    <x v="0"/>
+    <n v="13"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_46"/>
+    <x v="0"/>
+    <n v="2"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_47"/>
+    <x v="0"/>
+    <n v="6"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_48"/>
+    <x v="0"/>
+    <n v="5"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="2014_49"/>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_1"/>
+    <x v="2"/>
+    <s v="24"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_2"/>
+    <x v="2"/>
+    <s v="13"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_3"/>
+    <x v="2"/>
+    <s v="7"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_4"/>
+    <x v="2"/>
+    <s v="5"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_5"/>
+    <x v="2"/>
+    <s v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_6"/>
+    <x v="2"/>
+    <s v="9"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_7"/>
+    <x v="3"/>
+    <s v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_8"/>
+    <x v="2"/>
+    <s v="12"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_9"/>
+    <x v="3"/>
+    <s v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_10"/>
+    <x v="2"/>
+    <s v="1"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_11"/>
+    <x v="2"/>
+    <s v="1"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_12"/>
+    <x v="2"/>
+    <s v="19"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_13"/>
+    <x v="2"/>
+    <s v="10"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_14"/>
+    <x v="2"/>
+    <s v="2"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_15"/>
+    <x v="2"/>
+    <s v="7"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_16"/>
+    <x v="2"/>
+    <s v="4"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_17"/>
+    <x v="2"/>
+    <s v="14"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_18"/>
+    <x v="2"/>
+    <s v="4"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_19"/>
+    <x v="2"/>
+    <s v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_20"/>
+    <x v="2"/>
+    <s v="3"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_21"/>
+    <x v="3"/>
+    <s v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_22"/>
+    <x v="2"/>
+    <s v="9"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_23"/>
+    <x v="2"/>
+    <s v="4"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_24"/>
+    <x v="2"/>
+    <s v="6"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_25"/>
+    <x v="2"/>
+    <s v="3"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_26"/>
+    <x v="2"/>
+    <s v="9"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_27"/>
+    <x v="3"/>
+    <s v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_29"/>
+    <x v="2"/>
+    <s v="25"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_30"/>
+    <x v="2"/>
+    <s v="7"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_31"/>
+    <x v="3"/>
+    <s v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_32"/>
+    <x v="3"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_33"/>
+    <x v="2"/>
+    <s v="8"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_34"/>
+    <x v="2"/>
+    <s v="11"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_35"/>
+    <x v="2"/>
+    <s v="9"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_36"/>
+    <x v="3"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_37"/>
+    <x v="2"/>
+    <s v="9"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_38"/>
+    <x v="2"/>
+    <s v="8"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_39"/>
+    <x v="2"/>
+    <s v="7"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_40"/>
+    <x v="2"/>
+    <s v="7"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_41"/>
+    <x v="2"/>
+    <s v="2"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_42"/>
+    <x v="2"/>
+    <s v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_43"/>
+    <x v="3"/>
+    <s v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_45"/>
+    <x v="3"/>
+    <s v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_46"/>
+    <x v="3"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_47"/>
+    <x v="3"/>
+    <s v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_48"/>
+    <x v="3"/>
+    <s v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_49"/>
+    <x v="2"/>
+    <s v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_50"/>
+    <x v="2"/>
+    <s v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_51"/>
+    <x v="3"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="2015_52"/>
+    <x v="3"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <m/>
+    <x v="4"/>
+    <m/>
+    <x v="11"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:M8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" dataField="1" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="13">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="6"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of hunt.successful" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -865,8 +1988,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -876,7 +1999,7 @@
     <col min="6" max="16384" width="13.5" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>60</v>
       </c>
@@ -893,7 +2016,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>2013</v>
       </c>
@@ -910,7 +2033,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2013</v>
       </c>
@@ -927,7 +2050,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>2013</v>
       </c>
@@ -944,7 +2067,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>2013</v>
       </c>
@@ -961,7 +2084,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>2013</v>
       </c>
@@ -978,7 +2101,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>2013</v>
       </c>
@@ -1063,7 +2186,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>2013</v>
       </c>
@@ -1080,7 +2203,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>2013</v>
       </c>
@@ -1097,7 +2220,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>2013</v>
       </c>
@@ -1114,7 +2237,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>2013</v>
       </c>
@@ -1131,7 +2254,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>2013</v>
       </c>
@@ -1148,7 +2271,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>2013</v>
       </c>
@@ -1165,7 +2288,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>2013</v>
       </c>
@@ -1182,7 +2305,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>2013</v>
       </c>
@@ -1199,7 +2322,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>2013</v>
       </c>
@@ -1216,7 +2339,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>2013</v>
       </c>
@@ -1233,7 +2356,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>2013</v>
       </c>
@@ -1250,7 +2373,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>2013</v>
       </c>
@@ -1267,7 +2390,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>2013</v>
       </c>
@@ -1284,7 +2407,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>2013</v>
       </c>
@@ -1301,7 +2424,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>2013</v>
       </c>
@@ -1318,7 +2441,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>2013</v>
       </c>
@@ -1335,7 +2458,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>2013</v>
       </c>
@@ -1352,7 +2475,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>2013</v>
       </c>
@@ -1369,7 +2492,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>2013</v>
       </c>
@@ -1386,7 +2509,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>2013</v>
       </c>
@@ -1403,7 +2526,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>2013</v>
       </c>
@@ -1420,7 +2543,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>2013</v>
       </c>
@@ -1437,7 +2560,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>2014</v>
       </c>
@@ -1471,7 +2594,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>2014</v>
       </c>
@@ -1505,7 +2628,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>2014</v>
       </c>
@@ -1522,7 +2645,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>2014</v>
       </c>
@@ -1539,7 +2662,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>2014</v>
       </c>
@@ -1556,7 +2679,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>2014</v>
       </c>
@@ -1573,7 +2696,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>2014</v>
       </c>
@@ -1590,7 +2713,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>2014</v>
       </c>
@@ -1607,7 +2730,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>2014</v>
       </c>
@@ -1624,7 +2747,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>2014</v>
       </c>
@@ -1641,7 +2764,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>2014</v>
       </c>
@@ -1658,7 +2781,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>2014</v>
       </c>
@@ -1675,7 +2798,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>2014</v>
       </c>
@@ -1692,7 +2815,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>2014</v>
       </c>
@@ -1709,7 +2832,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>2014</v>
       </c>
@@ -1726,7 +2849,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>2014</v>
       </c>
@@ -1743,7 +2866,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>2014</v>
       </c>
@@ -1760,7 +2883,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>2014</v>
       </c>
@@ -1777,7 +2900,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>2014</v>
       </c>
@@ -1794,7 +2917,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>2014</v>
       </c>
@@ -1811,7 +2934,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>2014</v>
       </c>
@@ -1930,7 +3053,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>2014</v>
       </c>
@@ -1947,7 +3070,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>2014</v>
       </c>
@@ -1964,7 +3087,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>2014</v>
       </c>
@@ -1981,7 +3104,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>2014</v>
       </c>
@@ -1998,7 +3121,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>2014</v>
       </c>
@@ -2015,7 +3138,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>2014</v>
       </c>
@@ -2032,7 +3155,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>2014</v>
       </c>
@@ -2049,7 +3172,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>2014</v>
       </c>
@@ -2066,7 +3189,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>2014</v>
       </c>
@@ -2083,7 +3206,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>2014</v>
       </c>
@@ -2100,7 +3223,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>2014</v>
       </c>
@@ -2117,7 +3240,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>2014</v>
       </c>
@@ -2134,7 +3257,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>2014</v>
       </c>
@@ -2151,7 +3274,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>2014</v>
       </c>
@@ -2168,7 +3291,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>2014</v>
       </c>
@@ -2185,7 +3308,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>2014</v>
       </c>
@@ -2202,7 +3325,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>2014</v>
       </c>
@@ -2219,7 +3342,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="80" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>2014</v>
       </c>
@@ -2236,7 +3359,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>2014</v>
       </c>
@@ -2253,7 +3376,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>2014</v>
       </c>
@@ -2270,7 +3393,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="83" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="6">
         <v>2015</v>
       </c>
@@ -2287,7 +3410,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="84" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="6">
         <v>2015</v>
       </c>
@@ -2304,7 +3427,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="6">
         <v>2015</v>
       </c>
@@ -2321,7 +3444,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="6">
         <v>2015</v>
       </c>
@@ -2338,7 +3461,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="6">
         <v>2015</v>
       </c>
@@ -2355,7 +3478,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
         <v>2015</v>
       </c>
@@ -2389,7 +3512,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="6">
         <v>2015</v>
       </c>
@@ -2423,7 +3546,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
         <v>2015</v>
       </c>
@@ -2440,7 +3563,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="6">
         <v>2015</v>
       </c>
@@ -2457,7 +3580,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="6">
         <v>2015</v>
       </c>
@@ -2474,7 +3597,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="6">
         <v>2015</v>
       </c>
@@ -2491,7 +3614,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
         <v>2015</v>
       </c>
@@ -2508,7 +3631,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="6">
         <v>2015</v>
       </c>
@@ -2525,7 +3648,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
         <v>2015</v>
       </c>
@@ -2542,7 +3665,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="6">
         <v>2015</v>
       </c>
@@ -2559,7 +3682,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="6">
         <v>2015</v>
       </c>
@@ -2576,7 +3699,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="6">
         <v>2015</v>
       </c>
@@ -2593,7 +3716,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="6">
         <v>2015</v>
       </c>
@@ -2627,7 +3750,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="6">
         <v>2015</v>
       </c>
@@ -2644,7 +3767,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="6">
         <v>2015</v>
       </c>
@@ -2661,7 +3784,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="6">
         <v>2015</v>
       </c>
@@ -2678,7 +3801,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="6">
         <v>2015</v>
       </c>
@@ -2695,7 +3818,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="6">
         <v>2015</v>
       </c>
@@ -2729,7 +3852,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="6">
         <v>2015</v>
       </c>
@@ -2746,7 +3869,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="6">
         <v>2015</v>
       </c>
@@ -2797,7 +3920,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="6">
         <v>2015</v>
       </c>
@@ -2814,7 +3937,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="6">
         <v>2015</v>
       </c>
@@ -2831,7 +3954,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="6">
         <v>2015</v>
       </c>
@@ -2865,7 +3988,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="6">
         <v>2015</v>
       </c>
@@ -2882,7 +4005,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="119" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="6">
         <v>2015</v>
       </c>
@@ -2899,7 +4022,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="120" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="6">
         <v>2015</v>
       </c>
@@ -2916,7 +4039,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="6">
         <v>2015</v>
       </c>
@@ -2933,7 +4056,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="122" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="6">
         <v>2015</v>
       </c>
@@ -2950,7 +4073,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="6">
         <v>2015</v>
       </c>
@@ -3052,7 +4175,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="6">
         <v>2015</v>
       </c>
@@ -3069,7 +4192,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="6">
         <v>2015</v>
       </c>
@@ -3133,4 +4256,221 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.5" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" customWidth="1"/>
+    <col min="13" max="14" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" t="s">
+        <v>103</v>
+      </c>
+      <c r="M4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="10">
+        <v>5</v>
+      </c>
+      <c r="C5" s="10">
+        <v>12</v>
+      </c>
+      <c r="D5" s="10">
+        <v>6</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10">
+        <v>1</v>
+      </c>
+      <c r="L5" s="10">
+        <v>3</v>
+      </c>
+      <c r="M5" s="10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10">
+        <v>8</v>
+      </c>
+      <c r="G6" s="10">
+        <v>3</v>
+      </c>
+      <c r="H6" s="10">
+        <v>21</v>
+      </c>
+      <c r="I6" s="10">
+        <v>3</v>
+      </c>
+      <c r="J6" s="10">
+        <v>2</v>
+      </c>
+      <c r="K6" s="10">
+        <v>4</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>2015</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10">
+        <v>2</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10">
+        <v>15</v>
+      </c>
+      <c r="I7" s="10">
+        <v>14</v>
+      </c>
+      <c r="J7" s="10">
+        <v>2</v>
+      </c>
+      <c r="K7" s="10">
+        <v>3</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="10">
+        <v>5</v>
+      </c>
+      <c r="C8" s="10">
+        <v>12</v>
+      </c>
+      <c r="D8" s="10">
+        <v>6</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10">
+        <v>10</v>
+      </c>
+      <c r="G8" s="10">
+        <v>3</v>
+      </c>
+      <c r="H8" s="10">
+        <v>36</v>
+      </c>
+      <c r="I8" s="10">
+        <v>17</v>
+      </c>
+      <c r="J8" s="10">
+        <v>4</v>
+      </c>
+      <c r="K8" s="10">
+        <v>8</v>
+      </c>
+      <c r="L8" s="10">
+        <v>3</v>
+      </c>
+      <c r="M8" s="10">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>